<commit_message>
add: campo para guardar a sobrecarga
</commit_message>
<xml_diff>
--- a/trabalho1/transcoder/SimTranscoder/resultados/data.xlsx
+++ b/trabalho1/transcoder/SimTranscoder/resultados/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="tempo x instâncias" sheetId="1" r:id="rId1"/>
@@ -162,11 +162,11 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -268,82 +268,6 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'tempo x instâncias'!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>teste 1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'tempo x instâncias'!$A$5:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'tempo x instâncias'!$B$5:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4.9000000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.5999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.4000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7619</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7619</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
@@ -427,27 +351,27 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="117316416"/>
-        <c:axId val="117314456"/>
+        <c:axId val="194099048"/>
+        <c:axId val="194098264"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
+                <c:idx val="0"/>
+                <c:order val="0"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'tempo x instâncias'!$C$4</c15:sqref>
+                          <c15:sqref>'tempo x instâncias'!$B$4</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>teste 2</c:v>
+                        <c:v>teste 1</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -455,7 +379,7 @@
                 <c:spPr>
                   <a:ln w="19050" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -498,6 +422,102 @@
                   <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'tempo x instâncias'!$B$5:$B$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0000</c:formatCode>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>4.9000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4.5999999999999999E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>6.4000000000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>7619</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>7619</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'tempo x instâncias'!$C$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>teste 2</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'tempo x instâncias'!$A$5:$A$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>#,##0</c:formatCode>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>10000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>100000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'tempo x instâncias'!$C$5:$C$9</c15:sqref>
                         </c15:formulaRef>
@@ -819,7 +839,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="117316416"/>
+        <c:axId val="194099048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -932,12 +952,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117314456"/>
+        <c:crossAx val="194098264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="117314456"/>
+        <c:axId val="194098264"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1053,7 +1073,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117316416"/>
+        <c:crossAx val="194099048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1238,8 +1258,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="117317200"/>
-        <c:axId val="117317592"/>
+        <c:axId val="194097872"/>
+        <c:axId val="194093560"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1339,7 +1359,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117317200"/>
+        <c:axId val="194097872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1371,7 +1391,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1438,7 +1457,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117317592"/>
+        <c:crossAx val="194093560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1446,7 +1465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117317592"/>
+        <c:axId val="194093560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,7 +1579,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117317200"/>
+        <c:crossAx val="194097872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1574,7 +1593,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1821,8 +1839,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="317370096"/>
-        <c:axId val="317362648"/>
+        <c:axId val="194087680"/>
+        <c:axId val="194096696"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -2213,7 +2231,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="317370096"/>
+        <c:axId val="194087680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2326,12 +2344,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317362648"/>
+        <c:crossAx val="194096696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="317362648"/>
+        <c:axId val="194096696"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2447,7 +2465,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317370096"/>
+        <c:crossAx val="194087680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4347,8 +4365,8 @@
     <tableColumn id="3" name="teste 2" dataDxfId="4"/>
     <tableColumn id="4" name="teste 3" dataDxfId="3"/>
     <tableColumn id="5" name="teste 4" dataDxfId="2"/>
-    <tableColumn id="6" name="teste 5" dataDxfId="0"/>
-    <tableColumn id="7" name="MÉDIA (segundos):" dataDxfId="1">
+    <tableColumn id="6" name="teste 5" dataDxfId="1"/>
+    <tableColumn id="7" name="MÉDIA (segundos):" dataDxfId="0">
       <calculatedColumnFormula>AVERAGE(Tabela22[[#This Row],[teste 1]:[teste 5]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4646,8 +4664,8 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A4:M10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4949,7 +4967,7 @@
   <sheetPr codeName="Plan3"/>
   <dimension ref="A4:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>